<commit_message>
[23rd June 23]:- login Script designed
</commit_message>
<xml_diff>
--- a/TestData/SeleniumRevisionC'wad.xlsx
+++ b/TestData/SeleniumRevisionC'wad.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7988541d1216b5b/Desktop/Daily Examples/RevisionSession/Selenium/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC10481079DF4DE25ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44DF0457-77C9-4378-BFCB-20BA951462D7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83E00EC7-3997-40D7-A6AF-9E30E8FC8C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="abc" sheetId="3" r:id="rId3"/>
+    <sheet name="DDF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:E8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>abc</t>
   </si>
@@ -57,6 +53,9 @@
   </si>
   <si>
     <t>pdkqwd</t>
+  </si>
+  <si>
+    <t>Jan batch</t>
   </si>
 </sst>
 </file>
@@ -121,30 +120,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EC4042-E476-40E6-BA8F-F994202986E6}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,12 +504,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668692A-5649-4473-B42D-EA9DE28AA914}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated on 7July 2023
</commit_message>
<xml_diff>
--- a/TestData/SeleniumRevisionC'wad.xlsx
+++ b/TestData/SeleniumRevisionC'wad.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83E00EC7-3997-40D7-A6AF-9E30E8FC8C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="4410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="DDF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E8"/>
+  <oleSize ref="B1:H6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,13 +54,13 @@
     <t>pdkqwd</t>
   </si>
   <si>
-    <t>Jan batch</t>
+    <t>Jam batch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,19 +383,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -427,7 +426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
@@ -435,7 +434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100.5</v>
       </c>
@@ -443,30 +442,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" xr:uid="{AF270AAA-9554-47D3-9966-B8C864085BCE}"/>
+    <hyperlink ref="E1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EC4042-E476-40E6-BA8F-F994202986E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,17 +479,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -501,16 +500,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668692A-5649-4473-B42D-EA9DE28AA914}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>

</xml_diff>